<commit_message>
Finished EXT STD data code - needs more testing
</commit_message>
<xml_diff>
--- a/Ryan/FaOH_STDs/GCData_for_Ryan_w_FaOH_STD_Data.xlsx
+++ b/Ryan/FaOH_STDs/GCData_for_Ryan_w_FaOH_STD_Data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkong\Desktop\GitHub\GC_Code\Ryan\FaOH_STDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F3CCF-A134-4A9E-A3CA-F6AFA67422BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092FA3C1-A202-4BEF-AE92-49AF644511B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="John_Code" sheetId="1" r:id="rId1"/>
     <sheet name="Peak_ID" sheetId="2" r:id="rId2"/>
-    <sheet name="External_STD" sheetId="3" r:id="rId3"/>
-    <sheet name="Quantification w IS" sheetId="4" r:id="rId4"/>
-    <sheet name="Quantification w ES,IS" sheetId="5" r:id="rId5"/>
-    <sheet name="Data Output" sheetId="6" r:id="rId6"/>
-    <sheet name="Peak_ID (2)" sheetId="7" r:id="rId7"/>
+    <sheet name="Peak_ID (3)" sheetId="8" r:id="rId3"/>
+    <sheet name="External_STD" sheetId="3" r:id="rId4"/>
+    <sheet name="Quantification w IS" sheetId="4" r:id="rId5"/>
+    <sheet name="Quantification w ES,IS" sheetId="5" r:id="rId6"/>
+    <sheet name="Data Output" sheetId="6" r:id="rId7"/>
+    <sheet name="Peak_ID (2)" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="58">
   <si>
     <t>PeakNo</t>
   </si>
@@ -601,7 +602,7 @@
   <dimension ref="A1:F1621"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32180,7 +32181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -35501,6 +35504,4261 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:F212"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="F208" sqref="F208"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3.4460000000000002</v>
+      </c>
+      <c r="B2">
+        <v>3.379</v>
+      </c>
+      <c r="C2">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="D2">
+        <v>148050</v>
+      </c>
+      <c r="E2">
+        <v>36800</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.6440000000000001</v>
+      </c>
+      <c r="B3">
+        <v>4.5739999999999998</v>
+      </c>
+      <c r="C3">
+        <v>4.6859999999999999</v>
+      </c>
+      <c r="D3">
+        <v>460</v>
+      </c>
+      <c r="E3">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10.157999999999999</v>
+      </c>
+      <c r="B4">
+        <v>10.052</v>
+      </c>
+      <c r="C4">
+        <v>10.491</v>
+      </c>
+      <c r="D4">
+        <v>187457</v>
+      </c>
+      <c r="E4">
+        <v>46729</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12.436999999999999</v>
+      </c>
+      <c r="B5">
+        <v>12.375999999999999</v>
+      </c>
+      <c r="C5">
+        <v>12.605</v>
+      </c>
+      <c r="D5">
+        <v>189232</v>
+      </c>
+      <c r="E5">
+        <v>82739</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13.859</v>
+      </c>
+      <c r="B6">
+        <v>13.804</v>
+      </c>
+      <c r="C6">
+        <v>13.986000000000001</v>
+      </c>
+      <c r="D6">
+        <v>196642</v>
+      </c>
+      <c r="E6">
+        <v>100341</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.4369999999999998</v>
+      </c>
+      <c r="B8">
+        <v>3.36</v>
+      </c>
+      <c r="C8">
+        <v>3.64</v>
+      </c>
+      <c r="D8">
+        <v>103655</v>
+      </c>
+      <c r="E8">
+        <v>25676</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.99</v>
+      </c>
+      <c r="B9">
+        <v>5.8659999999999997</v>
+      </c>
+      <c r="C9">
+        <v>6.4359999999999999</v>
+      </c>
+      <c r="D9">
+        <v>130600</v>
+      </c>
+      <c r="E9">
+        <v>26693</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10.151</v>
+      </c>
+      <c r="B10">
+        <v>10.048</v>
+      </c>
+      <c r="C10">
+        <v>10.444000000000001</v>
+      </c>
+      <c r="D10">
+        <v>130163</v>
+      </c>
+      <c r="E10">
+        <v>32141</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12.433999999999999</v>
+      </c>
+      <c r="B11">
+        <v>12.381</v>
+      </c>
+      <c r="C11">
+        <v>12.6</v>
+      </c>
+      <c r="D11">
+        <v>119017</v>
+      </c>
+      <c r="E11">
+        <v>52537</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13.856999999999999</v>
+      </c>
+      <c r="B12">
+        <v>13.818</v>
+      </c>
+      <c r="C12">
+        <v>13.949</v>
+      </c>
+      <c r="D12">
+        <v>121718</v>
+      </c>
+      <c r="E12">
+        <v>64646</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.4430000000000001</v>
+      </c>
+      <c r="B14">
+        <v>3.379</v>
+      </c>
+      <c r="C14">
+        <v>3.6589999999999998</v>
+      </c>
+      <c r="D14">
+        <v>144970</v>
+      </c>
+      <c r="E14">
+        <v>34669</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.6459999999999999</v>
+      </c>
+      <c r="B15">
+        <v>4.5880000000000001</v>
+      </c>
+      <c r="C15">
+        <v>4.6719999999999997</v>
+      </c>
+      <c r="D15">
+        <v>368</v>
+      </c>
+      <c r="E15">
+        <v>133</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4.7140000000000004</v>
+      </c>
+      <c r="B16">
+        <v>4.6719999999999997</v>
+      </c>
+      <c r="C16">
+        <v>4.7839999999999998</v>
+      </c>
+      <c r="D16">
+        <v>436</v>
+      </c>
+      <c r="E16">
+        <v>115</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="B17">
+        <v>5.89</v>
+      </c>
+      <c r="C17">
+        <v>6.24</v>
+      </c>
+      <c r="D17">
+        <v>190124</v>
+      </c>
+      <c r="E17">
+        <v>38458</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10.157999999999999</v>
+      </c>
+      <c r="B18">
+        <v>10.061999999999999</v>
+      </c>
+      <c r="C18">
+        <v>10.519</v>
+      </c>
+      <c r="D18">
+        <v>195777</v>
+      </c>
+      <c r="E18">
+        <v>48396</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12.436</v>
+      </c>
+      <c r="B19">
+        <v>12.362</v>
+      </c>
+      <c r="C19">
+        <v>12.6</v>
+      </c>
+      <c r="D19">
+        <v>183344</v>
+      </c>
+      <c r="E19">
+        <v>80544</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="B20">
+        <v>13.818</v>
+      </c>
+      <c r="C20">
+        <v>14.005000000000001</v>
+      </c>
+      <c r="D20">
+        <v>190534</v>
+      </c>
+      <c r="E20">
+        <v>101742</v>
+      </c>
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3.4369999999999998</v>
+      </c>
+      <c r="B22">
+        <v>3.36</v>
+      </c>
+      <c r="C22">
+        <v>3.645</v>
+      </c>
+      <c r="D22">
+        <v>101936</v>
+      </c>
+      <c r="E22">
+        <v>26010</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4.6870000000000003</v>
+      </c>
+      <c r="B23">
+        <v>4.5590000000000002</v>
+      </c>
+      <c r="C23">
+        <v>4.7690000000000001</v>
+      </c>
+      <c r="D23">
+        <v>740</v>
+      </c>
+      <c r="E23">
+        <v>133</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5.992</v>
+      </c>
+      <c r="B24">
+        <v>5.875</v>
+      </c>
+      <c r="C24">
+        <v>6.319</v>
+      </c>
+      <c r="D24">
+        <v>118811</v>
+      </c>
+      <c r="E24">
+        <v>24670</v>
+      </c>
+      <c r="F24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10.153</v>
+      </c>
+      <c r="B25">
+        <v>10.057</v>
+      </c>
+      <c r="C25">
+        <v>10.435</v>
+      </c>
+      <c r="D25">
+        <v>117794</v>
+      </c>
+      <c r="E25">
+        <v>29596</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12.435</v>
+      </c>
+      <c r="B26">
+        <v>12.371</v>
+      </c>
+      <c r="C26">
+        <v>12.605</v>
+      </c>
+      <c r="D26">
+        <v>112527</v>
+      </c>
+      <c r="E26">
+        <v>50267</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="B27">
+        <v>13.818</v>
+      </c>
+      <c r="C27">
+        <v>14.023</v>
+      </c>
+      <c r="D27">
+        <v>117987</v>
+      </c>
+      <c r="E27">
+        <v>62978</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>14.433999999999999</v>
+      </c>
+      <c r="B28">
+        <v>14.294</v>
+      </c>
+      <c r="C28">
+        <v>14.457000000000001</v>
+      </c>
+      <c r="D28">
+        <v>2083</v>
+      </c>
+      <c r="E28">
+        <v>518</v>
+      </c>
+      <c r="F28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.4329999999999998</v>
+      </c>
+      <c r="B30">
+        <v>3.3559999999999999</v>
+      </c>
+      <c r="C30">
+        <v>3.64</v>
+      </c>
+      <c r="D30">
+        <v>100652</v>
+      </c>
+      <c r="E30">
+        <v>25408</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4.6740000000000004</v>
+      </c>
+      <c r="B31">
+        <v>4.6390000000000002</v>
+      </c>
+      <c r="C31">
+        <v>4.7649999999999997</v>
+      </c>
+      <c r="D31">
+        <v>480</v>
+      </c>
+      <c r="E31">
+        <v>132</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5.9880000000000004</v>
+      </c>
+      <c r="B32">
+        <v>5.8620000000000001</v>
+      </c>
+      <c r="C32">
+        <v>6.3049999999999997</v>
+      </c>
+      <c r="D32">
+        <v>113042</v>
+      </c>
+      <c r="E32">
+        <v>24006</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10.148</v>
+      </c>
+      <c r="B33">
+        <v>10.052</v>
+      </c>
+      <c r="C33">
+        <v>10.426</v>
+      </c>
+      <c r="D33">
+        <v>109329</v>
+      </c>
+      <c r="E33">
+        <v>27371</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>12.433999999999999</v>
+      </c>
+      <c r="B34">
+        <v>12.372</v>
+      </c>
+      <c r="C34">
+        <v>12.6</v>
+      </c>
+      <c r="D34">
+        <v>104202</v>
+      </c>
+      <c r="E34">
+        <v>46266</v>
+      </c>
+      <c r="F34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="B35">
+        <v>13.818</v>
+      </c>
+      <c r="C35">
+        <v>13.944000000000001</v>
+      </c>
+      <c r="D35">
+        <v>108745</v>
+      </c>
+      <c r="E35">
+        <v>58109</v>
+      </c>
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>14.435</v>
+      </c>
+      <c r="B36">
+        <v>14.304</v>
+      </c>
+      <c r="C36">
+        <v>14.452999999999999</v>
+      </c>
+      <c r="D36">
+        <v>2222</v>
+      </c>
+      <c r="E36">
+        <v>534</v>
+      </c>
+      <c r="F36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3.452</v>
+      </c>
+      <c r="B38">
+        <v>3.383</v>
+      </c>
+      <c r="C38">
+        <v>3.673</v>
+      </c>
+      <c r="D38">
+        <v>138124</v>
+      </c>
+      <c r="E38">
+        <v>31838</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4.6779999999999999</v>
+      </c>
+      <c r="B39">
+        <v>4.625</v>
+      </c>
+      <c r="C39">
+        <v>4.7270000000000003</v>
+      </c>
+      <c r="D39">
+        <v>715</v>
+      </c>
+      <c r="E39">
+        <v>177</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6.0090000000000003</v>
+      </c>
+      <c r="B40">
+        <v>5.9169999999999998</v>
+      </c>
+      <c r="C40">
+        <v>6.431</v>
+      </c>
+      <c r="D40">
+        <v>200123</v>
+      </c>
+      <c r="E40">
+        <v>37005</v>
+      </c>
+      <c r="F40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>10.17</v>
+      </c>
+      <c r="B41">
+        <v>10.047000000000001</v>
+      </c>
+      <c r="C41">
+        <v>10.494999999999999</v>
+      </c>
+      <c r="D41">
+        <v>213181</v>
+      </c>
+      <c r="E41">
+        <v>51170</v>
+      </c>
+      <c r="F41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>12.44</v>
+      </c>
+      <c r="B42">
+        <v>12.371</v>
+      </c>
+      <c r="C42">
+        <v>12.698</v>
+      </c>
+      <c r="D42">
+        <v>212420</v>
+      </c>
+      <c r="E42">
+        <v>95831</v>
+      </c>
+      <c r="F42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>13.86</v>
+      </c>
+      <c r="B43">
+        <v>13.813000000000001</v>
+      </c>
+      <c r="C43">
+        <v>13.972</v>
+      </c>
+      <c r="D43">
+        <v>224708</v>
+      </c>
+      <c r="E43">
+        <v>118182</v>
+      </c>
+      <c r="F43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>14.432</v>
+      </c>
+      <c r="B44">
+        <v>14.303000000000001</v>
+      </c>
+      <c r="C44">
+        <v>14.462</v>
+      </c>
+      <c r="D44">
+        <v>2661</v>
+      </c>
+      <c r="E44">
+        <v>865</v>
+      </c>
+      <c r="F44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3.444</v>
+      </c>
+      <c r="B46">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="C46">
+        <v>3.794</v>
+      </c>
+      <c r="D46">
+        <v>19664</v>
+      </c>
+      <c r="E46">
+        <v>3342</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="B47">
+        <v>4.4939999999999998</v>
+      </c>
+      <c r="C47">
+        <v>4.8209999999999997</v>
+      </c>
+      <c r="D47">
+        <v>12086</v>
+      </c>
+      <c r="E47">
+        <v>2784</v>
+      </c>
+      <c r="F47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>6.0149999999999997</v>
+      </c>
+      <c r="B48">
+        <v>5.931</v>
+      </c>
+      <c r="C48">
+        <v>6.2389999999999999</v>
+      </c>
+      <c r="D48">
+        <v>12220</v>
+      </c>
+      <c r="E48">
+        <v>2747</v>
+      </c>
+      <c r="F48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>7.9349999999999996</v>
+      </c>
+      <c r="B49">
+        <v>7.8310000000000004</v>
+      </c>
+      <c r="C49">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="D49">
+        <v>11364</v>
+      </c>
+      <c r="E49">
+        <v>2081</v>
+      </c>
+      <c r="F49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10.18</v>
+      </c>
+      <c r="B50">
+        <v>10.099</v>
+      </c>
+      <c r="C50">
+        <v>10.351000000000001</v>
+      </c>
+      <c r="D50">
+        <v>11354</v>
+      </c>
+      <c r="E50">
+        <v>3008</v>
+      </c>
+      <c r="F50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>11.499000000000001</v>
+      </c>
+      <c r="B51">
+        <v>11.438000000000001</v>
+      </c>
+      <c r="C51">
+        <v>11.625</v>
+      </c>
+      <c r="D51">
+        <v>11671</v>
+      </c>
+      <c r="E51">
+        <v>4306</v>
+      </c>
+      <c r="F51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>12.458</v>
+      </c>
+      <c r="B52">
+        <v>12.414</v>
+      </c>
+      <c r="C52">
+        <v>12.54</v>
+      </c>
+      <c r="D52">
+        <v>11474</v>
+      </c>
+      <c r="E52">
+        <v>5155</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>13.226000000000001</v>
+      </c>
+      <c r="B53">
+        <v>13.03</v>
+      </c>
+      <c r="C53">
+        <v>13.3</v>
+      </c>
+      <c r="D53">
+        <v>15509</v>
+      </c>
+      <c r="E53">
+        <v>5944</v>
+      </c>
+      <c r="F53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>13.875999999999999</v>
+      </c>
+      <c r="B54">
+        <v>13.523999999999999</v>
+      </c>
+      <c r="C54">
+        <v>13.944000000000001</v>
+      </c>
+      <c r="D54">
+        <v>47410</v>
+      </c>
+      <c r="E54">
+        <v>8153</v>
+      </c>
+      <c r="F54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>14.449</v>
+      </c>
+      <c r="B55">
+        <v>13.944000000000001</v>
+      </c>
+      <c r="C55">
+        <v>14.499000000000001</v>
+      </c>
+      <c r="D55">
+        <v>136275</v>
+      </c>
+      <c r="E55">
+        <v>11413</v>
+      </c>
+      <c r="F55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3.4180000000000001</v>
+      </c>
+      <c r="B57">
+        <v>3.379</v>
+      </c>
+      <c r="C57">
+        <v>3.556</v>
+      </c>
+      <c r="D57">
+        <v>1828</v>
+      </c>
+      <c r="E57">
+        <v>601</v>
+      </c>
+      <c r="F57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>6.0129999999999999</v>
+      </c>
+      <c r="B58">
+        <v>5.931</v>
+      </c>
+      <c r="C58">
+        <v>6.202</v>
+      </c>
+      <c r="D58">
+        <v>2363</v>
+      </c>
+      <c r="E58">
+        <v>447</v>
+      </c>
+      <c r="F58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>7.9429999999999996</v>
+      </c>
+      <c r="B59">
+        <v>7.8490000000000002</v>
+      </c>
+      <c r="C59">
+        <v>8.0879999999999992</v>
+      </c>
+      <c r="D59">
+        <v>2707</v>
+      </c>
+      <c r="E59">
+        <v>462</v>
+      </c>
+      <c r="F59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>10.186999999999999</v>
+      </c>
+      <c r="B60">
+        <v>10.118</v>
+      </c>
+      <c r="C60">
+        <v>10.304</v>
+      </c>
+      <c r="D60">
+        <v>4028</v>
+      </c>
+      <c r="E60">
+        <v>1051</v>
+      </c>
+      <c r="F60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>11.502000000000001</v>
+      </c>
+      <c r="B61">
+        <v>11.419</v>
+      </c>
+      <c r="C61">
+        <v>11.616</v>
+      </c>
+      <c r="D61">
+        <v>6151</v>
+      </c>
+      <c r="E61">
+        <v>2255</v>
+      </c>
+      <c r="F61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>12.461</v>
+      </c>
+      <c r="B62">
+        <v>12.134</v>
+      </c>
+      <c r="C62">
+        <v>12.544</v>
+      </c>
+      <c r="D62">
+        <v>8154</v>
+      </c>
+      <c r="E62">
+        <v>3667</v>
+      </c>
+      <c r="F62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>13.228</v>
+      </c>
+      <c r="B63">
+        <v>13.015000000000001</v>
+      </c>
+      <c r="C63">
+        <v>13.31</v>
+      </c>
+      <c r="D63">
+        <v>14350</v>
+      </c>
+      <c r="E63">
+        <v>5576</v>
+      </c>
+      <c r="F63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>13.878</v>
+      </c>
+      <c r="B64">
+        <v>13.706</v>
+      </c>
+      <c r="C64">
+        <v>13.949</v>
+      </c>
+      <c r="D64">
+        <v>37876</v>
+      </c>
+      <c r="E64">
+        <v>8991</v>
+      </c>
+      <c r="F64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>14.45</v>
+      </c>
+      <c r="B65">
+        <v>13.949</v>
+      </c>
+      <c r="C65">
+        <v>14.499000000000001</v>
+      </c>
+      <c r="D65">
+        <v>139815</v>
+      </c>
+      <c r="E65">
+        <v>13588</v>
+      </c>
+      <c r="F65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>3.468</v>
+      </c>
+      <c r="B67">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="C67">
+        <v>4.1909999999999998</v>
+      </c>
+      <c r="D67">
+        <v>2522844</v>
+      </c>
+      <c r="E67">
+        <v>748549</v>
+      </c>
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>4.6079999999999997</v>
+      </c>
+      <c r="B68">
+        <v>4.49</v>
+      </c>
+      <c r="C68">
+        <v>5.5069999999999997</v>
+      </c>
+      <c r="D68">
+        <v>2589475</v>
+      </c>
+      <c r="E68">
+        <v>678515</v>
+      </c>
+      <c r="F68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>6.0650000000000004</v>
+      </c>
+      <c r="B69">
+        <v>5.923</v>
+      </c>
+      <c r="C69">
+        <v>7.1449999999999996</v>
+      </c>
+      <c r="D69">
+        <v>2747118</v>
+      </c>
+      <c r="E69">
+        <v>640655</v>
+      </c>
+      <c r="F69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>8.02</v>
+      </c>
+      <c r="B70">
+        <v>7.8220000000000001</v>
+      </c>
+      <c r="C70">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="D70">
+        <v>2679104</v>
+      </c>
+      <c r="E70">
+        <v>473634</v>
+      </c>
+      <c r="F70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>10.244</v>
+      </c>
+      <c r="B71">
+        <v>10.118</v>
+      </c>
+      <c r="C71">
+        <v>11.378</v>
+      </c>
+      <c r="D71">
+        <v>2783594</v>
+      </c>
+      <c r="E71">
+        <v>707901</v>
+      </c>
+      <c r="F71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>11.548999999999999</v>
+      </c>
+      <c r="B72">
+        <v>11.382999999999999</v>
+      </c>
+      <c r="C72">
+        <v>12.409000000000001</v>
+      </c>
+      <c r="D72">
+        <v>2929293</v>
+      </c>
+      <c r="E72">
+        <v>986600</v>
+      </c>
+      <c r="F72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>12.502000000000001</v>
+      </c>
+      <c r="B73">
+        <v>12.414</v>
+      </c>
+      <c r="C73">
+        <v>13.151</v>
+      </c>
+      <c r="D73">
+        <v>3076296</v>
+      </c>
+      <c r="E73">
+        <v>1185638</v>
+      </c>
+      <c r="F73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>13.266</v>
+      </c>
+      <c r="B74">
+        <v>13.183999999999999</v>
+      </c>
+      <c r="C74">
+        <v>13.837</v>
+      </c>
+      <c r="D74">
+        <v>3113534</v>
+      </c>
+      <c r="E74">
+        <v>1298150</v>
+      </c>
+      <c r="F74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>13.776999999999999</v>
+      </c>
+      <c r="B75">
+        <v>13.753</v>
+      </c>
+      <c r="C75">
+        <v>13.837</v>
+      </c>
+      <c r="D75">
+        <v>13376</v>
+      </c>
+      <c r="E75">
+        <v>5979</v>
+      </c>
+      <c r="F75" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>13.914999999999999</v>
+      </c>
+      <c r="B76">
+        <v>13.837</v>
+      </c>
+      <c r="C76">
+        <v>13.987</v>
+      </c>
+      <c r="D76">
+        <v>3210020</v>
+      </c>
+      <c r="E76">
+        <v>1397360</v>
+      </c>
+      <c r="F76" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>14.484</v>
+      </c>
+      <c r="B77">
+        <v>14.313000000000001</v>
+      </c>
+      <c r="C77">
+        <v>14.92</v>
+      </c>
+      <c r="D77">
+        <v>3075718</v>
+      </c>
+      <c r="E77">
+        <v>1376753</v>
+      </c>
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="B79">
+        <v>3.3610000000000002</v>
+      </c>
+      <c r="C79">
+        <v>3.8780000000000001</v>
+      </c>
+      <c r="D79">
+        <v>102211</v>
+      </c>
+      <c r="E79">
+        <v>21475</v>
+      </c>
+      <c r="F79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>4.58</v>
+      </c>
+      <c r="B80">
+        <v>4.4850000000000003</v>
+      </c>
+      <c r="C80">
+        <v>4.8630000000000004</v>
+      </c>
+      <c r="D80">
+        <v>96901</v>
+      </c>
+      <c r="E80">
+        <v>22300</v>
+      </c>
+      <c r="F80" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>6.0209999999999999</v>
+      </c>
+      <c r="B81">
+        <v>5.9320000000000004</v>
+      </c>
+      <c r="C81">
+        <v>6.3559999999999999</v>
+      </c>
+      <c r="D81">
+        <v>109416</v>
+      </c>
+      <c r="E81">
+        <v>24854</v>
+      </c>
+      <c r="F81" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>7.944</v>
+      </c>
+      <c r="B82">
+        <v>7.8310000000000004</v>
+      </c>
+      <c r="C82">
+        <v>8.2889999999999997</v>
+      </c>
+      <c r="D82">
+        <v>112460</v>
+      </c>
+      <c r="E82">
+        <v>20421</v>
+      </c>
+      <c r="F82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>10.183999999999999</v>
+      </c>
+      <c r="B83">
+        <v>10.103999999999999</v>
+      </c>
+      <c r="C83">
+        <v>10.477</v>
+      </c>
+      <c r="D83">
+        <v>121218</v>
+      </c>
+      <c r="E83">
+        <v>32258</v>
+      </c>
+      <c r="F83" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>11.503</v>
+      </c>
+      <c r="B84">
+        <v>11.438000000000001</v>
+      </c>
+      <c r="C84">
+        <v>11.718999999999999</v>
+      </c>
+      <c r="D84">
+        <v>131328</v>
+      </c>
+      <c r="E84">
+        <v>49748</v>
+      </c>
+      <c r="F84" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>12.461</v>
+      </c>
+      <c r="B85">
+        <v>12.377000000000001</v>
+      </c>
+      <c r="C85">
+        <v>12.61</v>
+      </c>
+      <c r="D85">
+        <v>140772</v>
+      </c>
+      <c r="E85">
+        <v>62446</v>
+      </c>
+      <c r="F85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>13.228999999999999</v>
+      </c>
+      <c r="B86">
+        <v>13.151</v>
+      </c>
+      <c r="C86">
+        <v>13.342000000000001</v>
+      </c>
+      <c r="D86">
+        <v>143713</v>
+      </c>
+      <c r="E86">
+        <v>71951</v>
+      </c>
+      <c r="F86" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>13.771000000000001</v>
+      </c>
+      <c r="B87">
+        <v>13.739000000000001</v>
+      </c>
+      <c r="C87">
+        <v>13.791</v>
+      </c>
+      <c r="D87">
+        <v>1978</v>
+      </c>
+      <c r="E87">
+        <v>744</v>
+      </c>
+      <c r="F87" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>13.879</v>
+      </c>
+      <c r="B88">
+        <v>13.791</v>
+      </c>
+      <c r="C88">
+        <v>13.973000000000001</v>
+      </c>
+      <c r="D88">
+        <v>158776</v>
+      </c>
+      <c r="E88">
+        <v>81055</v>
+      </c>
+      <c r="F88" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>14.451000000000001</v>
+      </c>
+      <c r="B89">
+        <v>14.211</v>
+      </c>
+      <c r="C89">
+        <v>14.584</v>
+      </c>
+      <c r="D89">
+        <v>211310</v>
+      </c>
+      <c r="E89">
+        <v>80287</v>
+      </c>
+      <c r="F89" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" t="s">
+        <v>17</v>
+      </c>
+      <c r="F90" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>3.456</v>
+      </c>
+      <c r="B91">
+        <v>3.3559999999999999</v>
+      </c>
+      <c r="C91">
+        <v>4.1769999999999996</v>
+      </c>
+      <c r="D91">
+        <v>1177901</v>
+      </c>
+      <c r="E91">
+        <v>294663</v>
+      </c>
+      <c r="F91" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4.59</v>
+      </c>
+      <c r="B92">
+        <v>4.4850000000000003</v>
+      </c>
+      <c r="C92">
+        <v>5.47</v>
+      </c>
+      <c r="D92">
+        <v>1232414</v>
+      </c>
+      <c r="E92">
+        <v>298593</v>
+      </c>
+      <c r="F92" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>6.0389999999999997</v>
+      </c>
+      <c r="B93">
+        <v>5.9130000000000003</v>
+      </c>
+      <c r="C93">
+        <v>7.1449999999999996</v>
+      </c>
+      <c r="D93">
+        <v>1323017</v>
+      </c>
+      <c r="E93">
+        <v>305644</v>
+      </c>
+      <c r="F93" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>7.9790000000000001</v>
+      </c>
+      <c r="B94">
+        <v>7.8170000000000002</v>
+      </c>
+      <c r="C94">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="D94">
+        <v>1295064</v>
+      </c>
+      <c r="E94">
+        <v>238402</v>
+      </c>
+      <c r="F94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>10.215</v>
+      </c>
+      <c r="B95">
+        <v>10.113</v>
+      </c>
+      <c r="C95">
+        <v>11.448</v>
+      </c>
+      <c r="D95">
+        <v>1342950</v>
+      </c>
+      <c r="E95">
+        <v>368518</v>
+      </c>
+      <c r="F95" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>11.526999999999999</v>
+      </c>
+      <c r="B96">
+        <v>11.448</v>
+      </c>
+      <c r="C96">
+        <v>12.39</v>
+      </c>
+      <c r="D96">
+        <v>1417179</v>
+      </c>
+      <c r="E96">
+        <v>520412</v>
+      </c>
+      <c r="F96" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>12.483000000000001</v>
+      </c>
+      <c r="B97">
+        <v>12.4</v>
+      </c>
+      <c r="C97">
+        <v>13.141999999999999</v>
+      </c>
+      <c r="D97">
+        <v>1494950</v>
+      </c>
+      <c r="E97">
+        <v>636034</v>
+      </c>
+      <c r="F97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>13.249000000000001</v>
+      </c>
+      <c r="B98">
+        <v>13.141999999999999</v>
+      </c>
+      <c r="C98">
+        <v>13.823</v>
+      </c>
+      <c r="D98">
+        <v>1547138</v>
+      </c>
+      <c r="E98">
+        <v>686957</v>
+      </c>
+      <c r="F98" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>13.772</v>
+      </c>
+      <c r="B99">
+        <v>13.747999999999999</v>
+      </c>
+      <c r="C99">
+        <v>13.823</v>
+      </c>
+      <c r="D99">
+        <v>6028</v>
+      </c>
+      <c r="E99">
+        <v>2895</v>
+      </c>
+      <c r="F99" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>13.898999999999999</v>
+      </c>
+      <c r="B100">
+        <v>13.823</v>
+      </c>
+      <c r="C100">
+        <v>14.304</v>
+      </c>
+      <c r="D100">
+        <v>1660713</v>
+      </c>
+      <c r="E100">
+        <v>764604</v>
+      </c>
+      <c r="F100" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>14.468999999999999</v>
+      </c>
+      <c r="B101">
+        <v>14.304</v>
+      </c>
+      <c r="C101">
+        <v>14.616</v>
+      </c>
+      <c r="D101">
+        <v>1526528</v>
+      </c>
+      <c r="E101">
+        <v>747034</v>
+      </c>
+      <c r="F101" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>11.526</v>
+      </c>
+      <c r="B102">
+        <v>11.494999999999999</v>
+      </c>
+      <c r="C102">
+        <v>11.592000000000001</v>
+      </c>
+      <c r="D102">
+        <v>3050</v>
+      </c>
+      <c r="E102">
+        <v>1924</v>
+      </c>
+      <c r="F102" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>11.513</v>
+      </c>
+      <c r="B103">
+        <v>11.484999999999999</v>
+      </c>
+      <c r="C103">
+        <v>11.593</v>
+      </c>
+      <c r="D103">
+        <v>7476</v>
+      </c>
+      <c r="E103">
+        <v>4518</v>
+      </c>
+      <c r="F103" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" t="s">
+        <v>20</v>
+      </c>
+      <c r="D104" t="s">
+        <v>20</v>
+      </c>
+      <c r="E104" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="B105">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="C105">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="D105">
+        <v>153308</v>
+      </c>
+      <c r="E105">
+        <v>36443</v>
+      </c>
+      <c r="F105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>6.0049999999999999</v>
+      </c>
+      <c r="B106">
+        <v>5.9039999999999999</v>
+      </c>
+      <c r="C106">
+        <v>6.2489999999999997</v>
+      </c>
+      <c r="D106">
+        <v>188442</v>
+      </c>
+      <c r="E106">
+        <v>37250</v>
+      </c>
+      <c r="F106" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>10.166</v>
+      </c>
+      <c r="B107">
+        <v>10.038</v>
+      </c>
+      <c r="C107">
+        <v>10.449</v>
+      </c>
+      <c r="D107">
+        <v>199936</v>
+      </c>
+      <c r="E107">
+        <v>49483</v>
+      </c>
+      <c r="F107" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>12.439</v>
+      </c>
+      <c r="B108">
+        <v>12.385999999999999</v>
+      </c>
+      <c r="C108">
+        <v>12.61</v>
+      </c>
+      <c r="D108">
+        <v>194893</v>
+      </c>
+      <c r="E108">
+        <v>88230</v>
+      </c>
+      <c r="F108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>13.861000000000001</v>
+      </c>
+      <c r="B109">
+        <v>13.808999999999999</v>
+      </c>
+      <c r="C109">
+        <v>13.972</v>
+      </c>
+      <c r="D109">
+        <v>196024</v>
+      </c>
+      <c r="E109">
+        <v>103060</v>
+      </c>
+      <c r="F109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" t="s">
+        <v>21</v>
+      </c>
+      <c r="F110" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>3.4529999999999998</v>
+      </c>
+      <c r="B111">
+        <v>3.37</v>
+      </c>
+      <c r="C111">
+        <v>3.6680000000000001</v>
+      </c>
+      <c r="D111">
+        <v>181600</v>
+      </c>
+      <c r="E111">
+        <v>41801</v>
+      </c>
+      <c r="F111" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>4.67</v>
+      </c>
+      <c r="B112">
+        <v>4.6109999999999998</v>
+      </c>
+      <c r="C112">
+        <v>4.7050000000000001</v>
+      </c>
+      <c r="D112">
+        <v>552</v>
+      </c>
+      <c r="E112">
+        <v>164</v>
+      </c>
+      <c r="F112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>6.01</v>
+      </c>
+      <c r="B113">
+        <v>5.9089999999999998</v>
+      </c>
+      <c r="C113">
+        <v>6.2539999999999996</v>
+      </c>
+      <c r="D113">
+        <v>245715</v>
+      </c>
+      <c r="E113">
+        <v>47622</v>
+      </c>
+      <c r="F113" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>10.17</v>
+      </c>
+      <c r="B114">
+        <v>10.067</v>
+      </c>
+      <c r="C114">
+        <v>10.462999999999999</v>
+      </c>
+      <c r="D114">
+        <v>264111</v>
+      </c>
+      <c r="E114">
+        <v>65143</v>
+      </c>
+      <c r="F114" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>12.441000000000001</v>
+      </c>
+      <c r="B115">
+        <v>12.381</v>
+      </c>
+      <c r="C115">
+        <v>12.61</v>
+      </c>
+      <c r="D115">
+        <v>233669</v>
+      </c>
+      <c r="E115">
+        <v>100998</v>
+      </c>
+      <c r="F115" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>13.861000000000001</v>
+      </c>
+      <c r="B116">
+        <v>13.814</v>
+      </c>
+      <c r="C116">
+        <v>13.949</v>
+      </c>
+      <c r="D116">
+        <v>233107</v>
+      </c>
+      <c r="E116">
+        <v>124026</v>
+      </c>
+      <c r="F116" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>22</v>
+      </c>
+      <c r="B117" t="s">
+        <v>22</v>
+      </c>
+      <c r="C117" t="s">
+        <v>22</v>
+      </c>
+      <c r="D117" t="s">
+        <v>22</v>
+      </c>
+      <c r="E117" t="s">
+        <v>22</v>
+      </c>
+      <c r="F117" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>3.4550000000000001</v>
+      </c>
+      <c r="B118">
+        <v>3.2949999999999999</v>
+      </c>
+      <c r="C118">
+        <v>3.673</v>
+      </c>
+      <c r="D118">
+        <v>185483</v>
+      </c>
+      <c r="E118">
+        <v>40901</v>
+      </c>
+      <c r="F118" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>4.6820000000000004</v>
+      </c>
+      <c r="B119">
+        <v>4.63</v>
+      </c>
+      <c r="C119">
+        <v>4.7320000000000002</v>
+      </c>
+      <c r="D119">
+        <v>690</v>
+      </c>
+      <c r="E119">
+        <v>166</v>
+      </c>
+      <c r="F119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>6.0140000000000002</v>
+      </c>
+      <c r="B120">
+        <v>5.923</v>
+      </c>
+      <c r="C120">
+        <v>6.2309999999999999</v>
+      </c>
+      <c r="D120">
+        <v>214835</v>
+      </c>
+      <c r="E120">
+        <v>40625</v>
+      </c>
+      <c r="F120" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>10.172000000000001</v>
+      </c>
+      <c r="B121">
+        <v>10.061999999999999</v>
+      </c>
+      <c r="C121">
+        <v>10.481999999999999</v>
+      </c>
+      <c r="D121">
+        <v>214909</v>
+      </c>
+      <c r="E121">
+        <v>52070</v>
+      </c>
+      <c r="F121" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>12.441000000000001</v>
+      </c>
+      <c r="B122">
+        <v>12.381</v>
+      </c>
+      <c r="C122">
+        <v>12.615</v>
+      </c>
+      <c r="D122">
+        <v>196608</v>
+      </c>
+      <c r="E122">
+        <v>87761</v>
+      </c>
+      <c r="F122" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>13.86</v>
+      </c>
+      <c r="B123">
+        <v>13.814</v>
+      </c>
+      <c r="C123">
+        <v>13.962999999999999</v>
+      </c>
+      <c r="D123">
+        <v>196562</v>
+      </c>
+      <c r="E123">
+        <v>102781</v>
+      </c>
+      <c r="F123" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" t="s">
+        <v>23</v>
+      </c>
+      <c r="D124" t="s">
+        <v>23</v>
+      </c>
+      <c r="E124" t="s">
+        <v>23</v>
+      </c>
+      <c r="F124" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>3.456</v>
+      </c>
+      <c r="B125">
+        <v>3.3740000000000001</v>
+      </c>
+      <c r="C125">
+        <v>3.6819999999999999</v>
+      </c>
+      <c r="D125">
+        <v>172506</v>
+      </c>
+      <c r="E125">
+        <v>38428</v>
+      </c>
+      <c r="F125" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>4.577</v>
+      </c>
+      <c r="B126">
+        <v>4.4480000000000004</v>
+      </c>
+      <c r="C126">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="D126">
+        <v>194122</v>
+      </c>
+      <c r="E126">
+        <v>38514</v>
+      </c>
+      <c r="F126" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>6.0149999999999997</v>
+      </c>
+      <c r="B127">
+        <v>5.9219999999999997</v>
+      </c>
+      <c r="C127">
+        <v>6.2160000000000002</v>
+      </c>
+      <c r="D127">
+        <v>212754</v>
+      </c>
+      <c r="E127">
+        <v>39352</v>
+      </c>
+      <c r="F127" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>7.9370000000000003</v>
+      </c>
+      <c r="B128">
+        <v>7.78</v>
+      </c>
+      <c r="C128">
+        <v>8.4</v>
+      </c>
+      <c r="D128">
+        <v>192177</v>
+      </c>
+      <c r="E128">
+        <v>25962</v>
+      </c>
+      <c r="F128" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>10.173</v>
+      </c>
+      <c r="B129">
+        <v>10.071</v>
+      </c>
+      <c r="C129">
+        <v>10.449</v>
+      </c>
+      <c r="D129">
+        <v>219767</v>
+      </c>
+      <c r="E129">
+        <v>51356</v>
+      </c>
+      <c r="F129" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>11.483000000000001</v>
+      </c>
+      <c r="B130">
+        <v>11.41</v>
+      </c>
+      <c r="C130">
+        <v>11.657999999999999</v>
+      </c>
+      <c r="D130">
+        <v>186856</v>
+      </c>
+      <c r="E130">
+        <v>68811</v>
+      </c>
+      <c r="F130" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>12.44</v>
+      </c>
+      <c r="B131">
+        <v>12.385999999999999</v>
+      </c>
+      <c r="C131">
+        <v>12.61</v>
+      </c>
+      <c r="D131">
+        <v>214558</v>
+      </c>
+      <c r="E131">
+        <v>94596</v>
+      </c>
+      <c r="F131" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>13.207000000000001</v>
+      </c>
+      <c r="B132">
+        <v>13.16</v>
+      </c>
+      <c r="C132">
+        <v>13.319000000000001</v>
+      </c>
+      <c r="D132">
+        <v>173541</v>
+      </c>
+      <c r="E132">
+        <v>85396</v>
+      </c>
+      <c r="F132" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="B133">
+        <v>13.808999999999999</v>
+      </c>
+      <c r="C133">
+        <v>13.949</v>
+      </c>
+      <c r="D133">
+        <v>219545</v>
+      </c>
+      <c r="E133">
+        <v>119240</v>
+      </c>
+      <c r="F133" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>14.432</v>
+      </c>
+      <c r="B134">
+        <v>14.397</v>
+      </c>
+      <c r="C134">
+        <v>14.518000000000001</v>
+      </c>
+      <c r="D134">
+        <v>163779</v>
+      </c>
+      <c r="E134">
+        <v>91552</v>
+      </c>
+      <c r="F134" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>24</v>
+      </c>
+      <c r="B135" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" t="s">
+        <v>24</v>
+      </c>
+      <c r="D135" t="s">
+        <v>24</v>
+      </c>
+      <c r="E135" t="s">
+        <v>24</v>
+      </c>
+      <c r="F135" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>3.4489999999999998</v>
+      </c>
+      <c r="B136">
+        <v>3.355</v>
+      </c>
+      <c r="C136">
+        <v>3.6629999999999998</v>
+      </c>
+      <c r="D136">
+        <v>162714</v>
+      </c>
+      <c r="E136">
+        <v>36672</v>
+      </c>
+      <c r="F136" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>4.5679999999999996</v>
+      </c>
+      <c r="B137">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="C137">
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="D137">
+        <v>200070</v>
+      </c>
+      <c r="E137">
+        <v>40766</v>
+      </c>
+      <c r="F137" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>6.0049999999999999</v>
+      </c>
+      <c r="B138">
+        <v>5.9080000000000004</v>
+      </c>
+      <c r="C138">
+        <v>6.2670000000000003</v>
+      </c>
+      <c r="D138">
+        <v>210323</v>
+      </c>
+      <c r="E138">
+        <v>39585</v>
+      </c>
+      <c r="F138" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>7.9260000000000002</v>
+      </c>
+      <c r="B139">
+        <v>7.77</v>
+      </c>
+      <c r="C139">
+        <v>8.3949999999999996</v>
+      </c>
+      <c r="D139">
+        <v>198363</v>
+      </c>
+      <c r="E139">
+        <v>28641</v>
+      </c>
+      <c r="F139" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>10.164999999999999</v>
+      </c>
+      <c r="B140">
+        <v>10.066000000000001</v>
+      </c>
+      <c r="C140">
+        <v>10.449</v>
+      </c>
+      <c r="D140">
+        <v>211755</v>
+      </c>
+      <c r="E140">
+        <v>50875</v>
+      </c>
+      <c r="F140" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>11.478999999999999</v>
+      </c>
+      <c r="B141">
+        <v>11.414999999999999</v>
+      </c>
+      <c r="C141">
+        <v>11.667</v>
+      </c>
+      <c r="D141">
+        <v>193685</v>
+      </c>
+      <c r="E141">
+        <v>68911</v>
+      </c>
+      <c r="F141" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>12.436999999999999</v>
+      </c>
+      <c r="B142">
+        <v>12.375999999999999</v>
+      </c>
+      <c r="C142">
+        <v>12.609</v>
+      </c>
+      <c r="D142">
+        <v>206044</v>
+      </c>
+      <c r="E142">
+        <v>91273</v>
+      </c>
+      <c r="F142" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>13.206</v>
+      </c>
+      <c r="B143">
+        <v>13.16</v>
+      </c>
+      <c r="C143">
+        <v>13.319000000000001</v>
+      </c>
+      <c r="D143">
+        <v>180090</v>
+      </c>
+      <c r="E143">
+        <v>86822</v>
+      </c>
+      <c r="F143" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="B144">
+        <v>13.813000000000001</v>
+      </c>
+      <c r="C144">
+        <v>13.952999999999999</v>
+      </c>
+      <c r="D144">
+        <v>212654</v>
+      </c>
+      <c r="E144">
+        <v>115293</v>
+      </c>
+      <c r="F144" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>14.430999999999999</v>
+      </c>
+      <c r="B145">
+        <v>14.391999999999999</v>
+      </c>
+      <c r="C145">
+        <v>14.509</v>
+      </c>
+      <c r="D145">
+        <v>172623</v>
+      </c>
+      <c r="E145">
+        <v>97800</v>
+      </c>
+      <c r="F145" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>25</v>
+      </c>
+      <c r="B146" t="s">
+        <v>25</v>
+      </c>
+      <c r="C146" t="s">
+        <v>25</v>
+      </c>
+      <c r="D146" t="s">
+        <v>25</v>
+      </c>
+      <c r="E146" t="s">
+        <v>25</v>
+      </c>
+      <c r="F146" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>3.444</v>
+      </c>
+      <c r="B147">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="C147">
+        <v>3.6549999999999998</v>
+      </c>
+      <c r="D147">
+        <v>131546</v>
+      </c>
+      <c r="E147">
+        <v>31232</v>
+      </c>
+      <c r="F147" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>4.5640000000000001</v>
+      </c>
+      <c r="B148">
+        <v>4.4290000000000003</v>
+      </c>
+      <c r="C148">
+        <v>4.7839999999999998</v>
+      </c>
+      <c r="D148">
+        <v>167830</v>
+      </c>
+      <c r="E148">
+        <v>35261</v>
+      </c>
+      <c r="F148" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="B149">
+        <v>5.9039999999999999</v>
+      </c>
+      <c r="C149">
+        <v>6.2450000000000001</v>
+      </c>
+      <c r="D149">
+        <v>177734</v>
+      </c>
+      <c r="E149">
+        <v>34804</v>
+      </c>
+      <c r="F149" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="B150">
+        <v>7.7709999999999999</v>
+      </c>
+      <c r="C150">
+        <v>8.3490000000000002</v>
+      </c>
+      <c r="D150">
+        <v>181353</v>
+      </c>
+      <c r="E150">
+        <v>27550</v>
+      </c>
+      <c r="F150" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>10.157999999999999</v>
+      </c>
+      <c r="B151">
+        <v>10.067</v>
+      </c>
+      <c r="C151">
+        <v>10.426</v>
+      </c>
+      <c r="D151">
+        <v>193641</v>
+      </c>
+      <c r="E151">
+        <v>47095</v>
+      </c>
+      <c r="F151" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>11.475</v>
+      </c>
+      <c r="B152">
+        <v>11.406000000000001</v>
+      </c>
+      <c r="C152">
+        <v>11.663</v>
+      </c>
+      <c r="D152">
+        <v>194867</v>
+      </c>
+      <c r="E152">
+        <v>69660</v>
+      </c>
+      <c r="F152" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>12.435</v>
+      </c>
+      <c r="B153">
+        <v>12.381</v>
+      </c>
+      <c r="C153">
+        <v>12.601000000000001</v>
+      </c>
+      <c r="D153">
+        <v>194492</v>
+      </c>
+      <c r="E153">
+        <v>86282</v>
+      </c>
+      <c r="F153" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>13.205</v>
+      </c>
+      <c r="B154">
+        <v>13.114000000000001</v>
+      </c>
+      <c r="C154">
+        <v>13.319000000000001</v>
+      </c>
+      <c r="D154">
+        <v>190821</v>
+      </c>
+      <c r="E154">
+        <v>95724</v>
+      </c>
+      <c r="F154" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>13.856999999999999</v>
+      </c>
+      <c r="B155">
+        <v>13.808999999999999</v>
+      </c>
+      <c r="C155">
+        <v>13.954000000000001</v>
+      </c>
+      <c r="D155">
+        <v>202536</v>
+      </c>
+      <c r="E155">
+        <v>108233</v>
+      </c>
+      <c r="F155" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>14.430999999999999</v>
+      </c>
+      <c r="B156">
+        <v>14.393000000000001</v>
+      </c>
+      <c r="C156">
+        <v>14.513999999999999</v>
+      </c>
+      <c r="D156">
+        <v>185716</v>
+      </c>
+      <c r="E156">
+        <v>103795</v>
+      </c>
+      <c r="F156" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" t="s">
+        <v>26</v>
+      </c>
+      <c r="C157" t="s">
+        <v>26</v>
+      </c>
+      <c r="D157" t="s">
+        <v>26</v>
+      </c>
+      <c r="E157" t="s">
+        <v>26</v>
+      </c>
+      <c r="F157" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>3.4380000000000002</v>
+      </c>
+      <c r="B158">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="C158">
+        <v>3.645</v>
+      </c>
+      <c r="D158">
+        <v>106907</v>
+      </c>
+      <c r="E158">
+        <v>25838</v>
+      </c>
+      <c r="F158" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="B159">
+        <v>5.88</v>
+      </c>
+      <c r="C159">
+        <v>6.24</v>
+      </c>
+      <c r="D159">
+        <v>126880</v>
+      </c>
+      <c r="E159">
+        <v>26439</v>
+      </c>
+      <c r="F159" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>10.154999999999999</v>
+      </c>
+      <c r="B160">
+        <v>10.057</v>
+      </c>
+      <c r="C160">
+        <v>10.435</v>
+      </c>
+      <c r="D160">
+        <v>130236</v>
+      </c>
+      <c r="E160">
+        <v>32454</v>
+      </c>
+      <c r="F160" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>12.436</v>
+      </c>
+      <c r="B161">
+        <v>12.381</v>
+      </c>
+      <c r="C161">
+        <v>12.61</v>
+      </c>
+      <c r="D161">
+        <v>125522</v>
+      </c>
+      <c r="E161">
+        <v>55950</v>
+      </c>
+      <c r="F161" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>13.859</v>
+      </c>
+      <c r="B162">
+        <v>13.804</v>
+      </c>
+      <c r="C162">
+        <v>14.01</v>
+      </c>
+      <c r="D162">
+        <v>130941</v>
+      </c>
+      <c r="E162">
+        <v>65271</v>
+      </c>
+      <c r="F162" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>27</v>
+      </c>
+      <c r="B163" t="s">
+        <v>27</v>
+      </c>
+      <c r="C163" t="s">
+        <v>27</v>
+      </c>
+      <c r="D163" t="s">
+        <v>27</v>
+      </c>
+      <c r="E163" t="s">
+        <v>27</v>
+      </c>
+      <c r="F163" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>3.4540000000000002</v>
+      </c>
+      <c r="B164">
+        <v>3.37</v>
+      </c>
+      <c r="C164">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="D164">
+        <v>155039</v>
+      </c>
+      <c r="E164">
+        <v>34954</v>
+      </c>
+      <c r="F164" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>4.5780000000000003</v>
+      </c>
+      <c r="B165">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="C165">
+        <v>4.625</v>
+      </c>
+      <c r="D165">
+        <v>415</v>
+      </c>
+      <c r="E165">
+        <v>183</v>
+      </c>
+      <c r="F165" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>4.681</v>
+      </c>
+      <c r="B166">
+        <v>4.625</v>
+      </c>
+      <c r="C166">
+        <v>4.7229999999999999</v>
+      </c>
+      <c r="D166">
+        <v>644</v>
+      </c>
+      <c r="E166">
+        <v>166</v>
+      </c>
+      <c r="F166" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>6.0149999999999997</v>
+      </c>
+      <c r="B167">
+        <v>5.9219999999999997</v>
+      </c>
+      <c r="C167">
+        <v>6.2069999999999999</v>
+      </c>
+      <c r="D167">
+        <v>197266</v>
+      </c>
+      <c r="E167">
+        <v>37321</v>
+      </c>
+      <c r="F167" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>10.172000000000001</v>
+      </c>
+      <c r="B168">
+        <v>10.066000000000001</v>
+      </c>
+      <c r="C168">
+        <v>10.462999999999999</v>
+      </c>
+      <c r="D168">
+        <v>192520</v>
+      </c>
+      <c r="E168">
+        <v>46192</v>
+      </c>
+      <c r="F168" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>12.442</v>
+      </c>
+      <c r="B169">
+        <v>12.381</v>
+      </c>
+      <c r="C169">
+        <v>12.61</v>
+      </c>
+      <c r="D169">
+        <v>183659</v>
+      </c>
+      <c r="E169">
+        <v>81543</v>
+      </c>
+      <c r="F169" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>13.861000000000001</v>
+      </c>
+      <c r="B170">
+        <v>13.818</v>
+      </c>
+      <c r="C170">
+        <v>13.991</v>
+      </c>
+      <c r="D170">
+        <v>189480</v>
+      </c>
+      <c r="E170">
+        <v>100593</v>
+      </c>
+      <c r="F170" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>28</v>
+      </c>
+      <c r="B171" t="s">
+        <v>28</v>
+      </c>
+      <c r="C171" t="s">
+        <v>28</v>
+      </c>
+      <c r="D171" t="s">
+        <v>28</v>
+      </c>
+      <c r="E171" t="s">
+        <v>28</v>
+      </c>
+      <c r="F171" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>3.4489999999999998</v>
+      </c>
+      <c r="B172">
+        <v>3.3559999999999999</v>
+      </c>
+      <c r="C172">
+        <v>3.6589999999999998</v>
+      </c>
+      <c r="D172">
+        <v>171856</v>
+      </c>
+      <c r="E172">
+        <v>40943</v>
+      </c>
+      <c r="F172" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="B173">
+        <v>5.899</v>
+      </c>
+      <c r="C173">
+        <v>6.4080000000000004</v>
+      </c>
+      <c r="D173">
+        <v>201164</v>
+      </c>
+      <c r="E173">
+        <v>39873</v>
+      </c>
+      <c r="F173" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>10.162000000000001</v>
+      </c>
+      <c r="B174">
+        <v>10.057</v>
+      </c>
+      <c r="C174">
+        <v>10.454000000000001</v>
+      </c>
+      <c r="D174">
+        <v>199497</v>
+      </c>
+      <c r="E174">
+        <v>49588</v>
+      </c>
+      <c r="F174" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>12.439</v>
+      </c>
+      <c r="B175">
+        <v>12.377000000000001</v>
+      </c>
+      <c r="C175">
+        <v>12.61</v>
+      </c>
+      <c r="D175">
+        <v>182108</v>
+      </c>
+      <c r="E175">
+        <v>80583</v>
+      </c>
+      <c r="F175" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>13.86</v>
+      </c>
+      <c r="B176">
+        <v>13.819000000000001</v>
+      </c>
+      <c r="C176">
+        <v>13.973000000000001</v>
+      </c>
+      <c r="D176">
+        <v>179919</v>
+      </c>
+      <c r="E176">
+        <v>93889</v>
+      </c>
+      <c r="F176" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>14.349</v>
+      </c>
+      <c r="B177">
+        <v>14.323</v>
+      </c>
+      <c r="C177">
+        <v>14.388</v>
+      </c>
+      <c r="D177">
+        <v>2115</v>
+      </c>
+      <c r="E177">
+        <v>1239</v>
+      </c>
+      <c r="F177" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>29</v>
+      </c>
+      <c r="B178" t="s">
+        <v>29</v>
+      </c>
+      <c r="C178" t="s">
+        <v>29</v>
+      </c>
+      <c r="D178" t="s">
+        <v>29</v>
+      </c>
+      <c r="E178" t="s">
+        <v>29</v>
+      </c>
+      <c r="F178" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>3.4550000000000001</v>
+      </c>
+      <c r="B179">
+        <v>3.3740000000000001</v>
+      </c>
+      <c r="C179">
+        <v>3.6539999999999999</v>
+      </c>
+      <c r="D179">
+        <v>163222</v>
+      </c>
+      <c r="E179">
+        <v>37025</v>
+      </c>
+      <c r="F179" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>4.5789999999999997</v>
+      </c>
+      <c r="B180">
+        <v>4.452</v>
+      </c>
+      <c r="C180">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="D180">
+        <v>726092</v>
+      </c>
+      <c r="E180">
+        <v>148680</v>
+      </c>
+      <c r="F180" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>6.0129999999999999</v>
+      </c>
+      <c r="B181">
+        <v>5.9180000000000001</v>
+      </c>
+      <c r="C181">
+        <v>6.2859999999999996</v>
+      </c>
+      <c r="D181">
+        <v>210846</v>
+      </c>
+      <c r="E181">
+        <v>38791</v>
+      </c>
+      <c r="F181" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>7.9779999999999998</v>
+      </c>
+      <c r="B182">
+        <v>7.78</v>
+      </c>
+      <c r="C182">
+        <v>8.5030000000000001</v>
+      </c>
+      <c r="D182">
+        <v>2602373</v>
+      </c>
+      <c r="E182">
+        <v>367231</v>
+      </c>
+      <c r="F182" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>10.173999999999999</v>
+      </c>
+      <c r="B183">
+        <v>10.023999999999999</v>
+      </c>
+      <c r="C183">
+        <v>10.412000000000001</v>
+      </c>
+      <c r="D183">
+        <v>211112</v>
+      </c>
+      <c r="E183">
+        <v>50266</v>
+      </c>
+      <c r="F183" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>11.525</v>
+      </c>
+      <c r="B184">
+        <v>11.414999999999999</v>
+      </c>
+      <c r="C184">
+        <v>11.662000000000001</v>
+      </c>
+      <c r="D184">
+        <v>3431965</v>
+      </c>
+      <c r="E184">
+        <v>1051299</v>
+      </c>
+      <c r="F184" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>12.441000000000001</v>
+      </c>
+      <c r="B185">
+        <v>12.381</v>
+      </c>
+      <c r="C185">
+        <v>12.577</v>
+      </c>
+      <c r="D185">
+        <v>203716</v>
+      </c>
+      <c r="E185">
+        <v>87985</v>
+      </c>
+      <c r="F185" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>13.233000000000001</v>
+      </c>
+      <c r="B186">
+        <v>13.16</v>
+      </c>
+      <c r="C186">
+        <v>13.337999999999999</v>
+      </c>
+      <c r="D186">
+        <v>2171436</v>
+      </c>
+      <c r="E186">
+        <v>958860</v>
+      </c>
+      <c r="F186" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>13.86</v>
+      </c>
+      <c r="B187">
+        <v>13.823</v>
+      </c>
+      <c r="C187">
+        <v>13.962999999999999</v>
+      </c>
+      <c r="D187">
+        <v>217729</v>
+      </c>
+      <c r="E187">
+        <v>112506</v>
+      </c>
+      <c r="F187" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>14.318</v>
+      </c>
+      <c r="B188">
+        <v>14.243</v>
+      </c>
+      <c r="C188">
+        <v>14.340999999999999</v>
+      </c>
+      <c r="D188">
+        <v>1559</v>
+      </c>
+      <c r="E188">
+        <v>405</v>
+      </c>
+      <c r="F188" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>14.436999999999999</v>
+      </c>
+      <c r="B189">
+        <v>14.397</v>
+      </c>
+      <c r="C189">
+        <v>14.523</v>
+      </c>
+      <c r="D189">
+        <v>407922</v>
+      </c>
+      <c r="E189">
+        <v>233256</v>
+      </c>
+      <c r="F189" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>30</v>
+      </c>
+      <c r="B190" t="s">
+        <v>30</v>
+      </c>
+      <c r="C190" t="s">
+        <v>30</v>
+      </c>
+      <c r="D190" t="s">
+        <v>30</v>
+      </c>
+      <c r="E190" t="s">
+        <v>30</v>
+      </c>
+      <c r="F190" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>3.4329999999999998</v>
+      </c>
+      <c r="B191">
+        <v>3.3559999999999999</v>
+      </c>
+      <c r="C191">
+        <v>3.6309999999999998</v>
+      </c>
+      <c r="D191">
+        <v>108413</v>
+      </c>
+      <c r="E191">
+        <v>26712</v>
+      </c>
+      <c r="F191" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>5.9870000000000001</v>
+      </c>
+      <c r="B192">
+        <v>5.89</v>
+      </c>
+      <c r="C192">
+        <v>6.1980000000000004</v>
+      </c>
+      <c r="D192">
+        <v>117770</v>
+      </c>
+      <c r="E192">
+        <v>24954</v>
+      </c>
+      <c r="F192" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>7.9210000000000003</v>
+      </c>
+      <c r="B193">
+        <v>7.7519999999999998</v>
+      </c>
+      <c r="C193">
+        <v>8.6850000000000005</v>
+      </c>
+      <c r="D193">
+        <v>1157917</v>
+      </c>
+      <c r="E193">
+        <v>196312</v>
+      </c>
+      <c r="F193" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>10.147</v>
+      </c>
+      <c r="B194">
+        <v>10.061999999999999</v>
+      </c>
+      <c r="C194">
+        <v>10.388</v>
+      </c>
+      <c r="D194">
+        <v>113969</v>
+      </c>
+      <c r="E194">
+        <v>28666</v>
+      </c>
+      <c r="F194" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>11.492000000000001</v>
+      </c>
+      <c r="B195">
+        <v>11.396000000000001</v>
+      </c>
+      <c r="C195">
+        <v>11.662000000000001</v>
+      </c>
+      <c r="D195">
+        <v>1478297</v>
+      </c>
+      <c r="E195">
+        <v>526604</v>
+      </c>
+      <c r="F195" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>12.433</v>
+      </c>
+      <c r="B196">
+        <v>12.385999999999999</v>
+      </c>
+      <c r="C196">
+        <v>12.571999999999999</v>
+      </c>
+      <c r="D196">
+        <v>108971</v>
+      </c>
+      <c r="E196">
+        <v>48250</v>
+      </c>
+      <c r="F196" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>13.215999999999999</v>
+      </c>
+      <c r="B197">
+        <v>13.156000000000001</v>
+      </c>
+      <c r="C197">
+        <v>13.333</v>
+      </c>
+      <c r="D197">
+        <v>941322</v>
+      </c>
+      <c r="E197">
+        <v>451132</v>
+      </c>
+      <c r="F197" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>13.856999999999999</v>
+      </c>
+      <c r="B198">
+        <v>13.818</v>
+      </c>
+      <c r="C198">
+        <v>13.962999999999999</v>
+      </c>
+      <c r="D198">
+        <v>113009</v>
+      </c>
+      <c r="E198">
+        <v>61128</v>
+      </c>
+      <c r="F198" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>14.318</v>
+      </c>
+      <c r="B199">
+        <v>14.238</v>
+      </c>
+      <c r="C199">
+        <v>14.336</v>
+      </c>
+      <c r="D199">
+        <v>588</v>
+      </c>
+      <c r="E199">
+        <v>159</v>
+      </c>
+      <c r="F199" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>14.433</v>
+      </c>
+      <c r="B200">
+        <v>14.397</v>
+      </c>
+      <c r="C200">
+        <v>14.523</v>
+      </c>
+      <c r="D200">
+        <v>180396</v>
+      </c>
+      <c r="E200">
+        <v>101573</v>
+      </c>
+      <c r="F200" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>31</v>
+      </c>
+      <c r="B201" t="s">
+        <v>31</v>
+      </c>
+      <c r="C201" t="s">
+        <v>31</v>
+      </c>
+      <c r="D201" t="s">
+        <v>31</v>
+      </c>
+      <c r="E201" t="s">
+        <v>31</v>
+      </c>
+      <c r="F201" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>3.4569999999999999</v>
+      </c>
+      <c r="B202">
+        <v>3.3</v>
+      </c>
+      <c r="C202">
+        <v>3.673</v>
+      </c>
+      <c r="D202">
+        <v>188787</v>
+      </c>
+      <c r="E202">
+        <v>41877</v>
+      </c>
+      <c r="F202" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>4.5739999999999998</v>
+      </c>
+      <c r="B203">
+        <v>4.42</v>
+      </c>
+      <c r="C203">
+        <v>4.798</v>
+      </c>
+      <c r="D203">
+        <v>15782</v>
+      </c>
+      <c r="E203">
+        <v>2869</v>
+      </c>
+      <c r="F203" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>6.0129999999999999</v>
+      </c>
+      <c r="B204">
+        <v>5.9219999999999997</v>
+      </c>
+      <c r="C204">
+        <v>6.2770000000000001</v>
+      </c>
+      <c r="D204">
+        <v>253048</v>
+      </c>
+      <c r="E204">
+        <v>48149</v>
+      </c>
+      <c r="F204" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>7.9329999999999998</v>
+      </c>
+      <c r="B205">
+        <v>7.7889999999999997</v>
+      </c>
+      <c r="C205">
+        <v>8.1809999999999992</v>
+      </c>
+      <c r="D205">
+        <v>39957</v>
+      </c>
+      <c r="E205">
+        <v>5601</v>
+      </c>
+      <c r="F205" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>10.172000000000001</v>
+      </c>
+      <c r="B206">
+        <v>10.066000000000001</v>
+      </c>
+      <c r="C206">
+        <v>10.416</v>
+      </c>
+      <c r="D206">
+        <v>263936</v>
+      </c>
+      <c r="E206">
+        <v>62788</v>
+      </c>
+      <c r="F206" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>11.48</v>
+      </c>
+      <c r="B207">
+        <v>11.387</v>
+      </c>
+      <c r="C207">
+        <v>11.63</v>
+      </c>
+      <c r="D207">
+        <v>54176</v>
+      </c>
+      <c r="E207">
+        <v>19398</v>
+      </c>
+      <c r="F207" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>12.44</v>
+      </c>
+      <c r="B208">
+        <v>12.381</v>
+      </c>
+      <c r="C208">
+        <v>12.577</v>
+      </c>
+      <c r="D208">
+        <v>227608</v>
+      </c>
+      <c r="E208">
+        <v>102253</v>
+      </c>
+      <c r="F208" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>13.205</v>
+      </c>
+      <c r="B209">
+        <v>13.16</v>
+      </c>
+      <c r="C209">
+        <v>13.305</v>
+      </c>
+      <c r="D209">
+        <v>33394</v>
+      </c>
+      <c r="E209">
+        <v>16501</v>
+      </c>
+      <c r="F209" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>13.859</v>
+      </c>
+      <c r="B210">
+        <v>13.818</v>
+      </c>
+      <c r="C210">
+        <v>13.962999999999999</v>
+      </c>
+      <c r="D210">
+        <v>209316</v>
+      </c>
+      <c r="E210">
+        <v>112921</v>
+      </c>
+      <c r="F210" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>14.346</v>
+      </c>
+      <c r="B211">
+        <v>14.318</v>
+      </c>
+      <c r="C211">
+        <v>14.397</v>
+      </c>
+      <c r="D211">
+        <v>8332</v>
+      </c>
+      <c r="E211">
+        <v>4726</v>
+      </c>
+      <c r="F211" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>14.429</v>
+      </c>
+      <c r="B212">
+        <v>14.397</v>
+      </c>
+      <c r="C212">
+        <v>14.476000000000001</v>
+      </c>
+      <c r="D212">
+        <v>6730</v>
+      </c>
+      <c r="E212">
+        <v>3560</v>
+      </c>
+      <c r="F212" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -35595,7 +39853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J211"/>
   <sheetViews>
@@ -39293,7 +43551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z211"/>
   <sheetViews>
@@ -43878,7 +48136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
@@ -44785,11 +49043,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>